<commit_message>
fixed a couple of words in the abstract
</commit_message>
<xml_diff>
--- a/reports/final/results.xlsx
+++ b/reports/final/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23780" windowHeight="15220" tabRatio="500"/>
+    <workbookView xWindow="8820" yWindow="980" windowWidth="23780" windowHeight="15220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -271,16 +271,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -624,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C9"/>
+  <dimension ref="B2:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -699,6 +699,41 @@
         <v>1</v>
       </c>
     </row>
+    <row r="17" spans="2:2">
+      <c r="B17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23">
+        <v>10000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>